<commit_message>
fix test import order
</commit_message>
<xml_diff>
--- a/operate/business/test/data/partnerOrder/TB_Orders.xlsx
+++ b/operate/business/test/data/partnerOrder/TB_Orders.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="560" yWindow="1640" windowWidth="25040" windowHeight="14420" tabRatio="500"/>
+    <workbookView xWindow="8340" yWindow="2900" windowWidth="25040" windowHeight="14060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>外部商品ID</t>
   </si>
@@ -57,32 +57,41 @@
     <t>送货地址</t>
   </si>
   <si>
+    <t>199201934887701</t>
+  </si>
+  <si>
+    <t>2013-01-07 10:52</t>
+  </si>
+  <si>
+    <t>江苏苏州市昆山市千灯镇少卿西路卿峰丽景南区苏式建筑198幢</t>
+  </si>
+  <si>
+    <t>益菱</t>
+  </si>
+  <si>
+    <t>13862393981</t>
+  </si>
+  <si>
+    <t>江苏苏州市昆山市(周庄、锦溪、淀山湖、千灯、张浦、陆家、花桥)江苏苏州市昆山市(周庄、锦溪、淀山湖、千灯、张浦、陆家、花桥)周庄锦溪淀山湖千灯张浦陆家花桥千灯镇少卿西路卿峰丽景南区苏式建筑198幢</t>
+  </si>
+  <si>
+    <t>199201934887701</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>23020076245</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>23020076246</t>
-  </si>
-  <si>
-    <t>199201934887701</t>
-  </si>
-  <si>
-    <t>2013-01-07 10:52</t>
-  </si>
-  <si>
-    <t>江苏苏州市昆山市千灯镇少卿西路卿峰丽景南区苏式建筑198幢</t>
-  </si>
-  <si>
-    <t>益菱</t>
-  </si>
-  <si>
-    <t>13862393981</t>
-  </si>
-  <si>
-    <t>江苏苏州市昆山市(周庄、锦溪、淀山湖、千灯、张浦、陆家、花桥)江苏苏州市昆山市(周庄、锦溪、淀山湖、千灯、张浦、陆家、花桥)周庄锦溪淀山湖千灯张浦陆家花桥千灯镇少卿西路卿峰丽景南区苏式建筑198幢</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -100,6 +109,18 @@
     </font>
     <font>
       <sz val="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="11"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -150,8 +171,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -164,7 +189,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="超链接" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="访问过的超链接" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="普通" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -494,9 +523,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="13.5" customHeight="1" x14ac:dyDescent="0"/>
   <cols>
@@ -545,10 +576,10 @@
     </row>
     <row r="2" spans="1:12" ht="213.75" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>465</v>
@@ -557,27 +588,60 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" s="2"/>
       <c r="I2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="213.75" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>18</v>
+      </c>
+      <c r="C3" s="2">
+        <v>465</v>
+      </c>
+      <c r="D3" s="2">
+        <v>2</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>